<commit_message>
new part sonarlint 1/2
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daria\OneDrive\Desktop\VVSS-labs\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8775474af38bcd54/Desktop/anul3/VVSS/VVSS-labs/Docs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F4FD46-6DA1-44A7-A17B-8F11551B1C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{99F4FD46-6DA1-44A7-A17B-8F11551B1C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80B598AF-E07D-4100-A9B9-D5F34FD486CA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -19,11 +19,24 @@
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -169,14 +182,204 @@
     <t>C04</t>
   </si>
   <si>
-    <t>Dacă structura fișierelor se schimbă sau dacă există erori în datele de intrare, codul actual nu trateaza aceste probleme într-un mod care să împiedice crash-ul aplicației sau erori de runtime. Ar trebui să existe validări ale formatului datelor citite.</t>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">gestionarea excepțiilor pentru </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IOException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e.printStackTrace();</t>
+    </r>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>In Kitchen GUI Controller avem un while (true) care ar putea fi inlocuit</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Metoda </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>getPayment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nu validează formatul datelor din fișier. Dacă linia citită nu respectă formatul așteptat, pot rezulta excepții runtime</t>
+    </r>
+  </si>
+  <si>
+    <t>Dacă structura fișierelDor se schimbă sau dacă există erori în datele de intrare, codul actual nu trateaza aceste probleme într-un mod care să împiedice crash-ul aplicației sau erori de runtime. Ar trebui să existe validări ale formatului datelor citite.</t>
+  </si>
+  <si>
+    <t>OrdersGUIController, 53</t>
+  </si>
+  <si>
+    <t>Make the enclosing method "static" or remove this set.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public void </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF56A8F5"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>setTotalAmount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCF8E6D"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">double </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>totalAmount) {</t>
+    </r>
+  </si>
+  <si>
+    <t>public static ….</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">try </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    br = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCF8E6D"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>BufferedReader(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCF8E6D"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>FileReader(file));</t>
+    </r>
+  </si>
+  <si>
+    <t>use try-with-resources</t>
+  </si>
+  <si>
+    <t>MenuRepository</t>
+  </si>
+  <si>
+    <t>Define a constant instead of duplicating this literal "--------------------------" 6 times.</t>
+  </si>
+  <si>
+    <t>PAymentAlert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +463,48 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFCF8E6D"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF56A8F5"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -361,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,6 +679,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,6 +705,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -743,23 +1003,23 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="6"/>
-    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.36328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.36328125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.81640625" style="6"/>
+    <col min="1" max="1" width="8.796875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.796875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.36328125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.81640625" style="6"/>
+    <col min="10" max="10" width="14.33203125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -770,7 +1030,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="B2" s="24" t="s">
         <v>19</v>
       </c>
@@ -785,7 +1045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -796,7 +1056,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -814,7 +1074,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
@@ -828,7 +1088,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -836,14 +1096,14 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -857,7 +1117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -869,7 +1129,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -882,7 +1142,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -895,7 +1155,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -904,7 +1164,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -913,7 +1173,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -922,7 +1182,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -931,7 +1191,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -940,7 +1200,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -949,7 +1209,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -958,7 +1218,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -967,7 +1227,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -976,7 +1236,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -985,7 +1245,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -994,7 +1254,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1003,7 +1263,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1012,13 +1272,13 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1042,22 +1302,22 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="6"/>
-    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.36328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.36328125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.81640625" style="6"/>
-    <col min="9" max="9" width="22.08984375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="6"/>
+    <col min="1" max="1" width="8.796875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.796875" style="6"/>
+    <col min="9" max="9" width="22.06640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1068,7 +1328,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
@@ -1083,7 +1343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1094,7 +1354,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1372,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +1386,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1134,14 +1394,14 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1155,7 +1415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1167,7 +1427,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1180,7 +1440,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1193,7 +1453,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1202,7 +1462,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1211,7 +1471,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1220,7 +1480,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1229,7 +1489,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1238,7 +1498,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1247,7 +1507,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1256,7 +1516,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1265,7 +1525,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1274,7 +1534,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1283,7 +1543,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1292,7 +1552,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1301,7 +1561,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1310,7 +1570,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1319,13 +1579,13 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1349,23 +1609,23 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="6"/>
-    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.36328125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.81640625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="6"/>
+    <col min="5" max="5" width="41.33203125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.796875" style="6"/>
+    <col min="9" max="9" width="26.73046875" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1376,7 +1636,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
@@ -1391,7 +1651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1402,7 +1662,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
@@ -1420,7 +1680,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -1434,7 +1694,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1442,14 +1702,14 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1463,7 +1723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1472,37 +1732,51 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E11" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E12" s="36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.5">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E13" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1511,7 +1785,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1520,7 +1794,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1529,7 +1803,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1538,7 +1812,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1547,7 +1821,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1556,7 +1830,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1565,7 +1839,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1574,7 +1848,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1583,7 +1857,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1592,7 +1866,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1601,7 +1875,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1610,7 +1884,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1619,7 +1893,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1628,7 +1902,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1637,7 +1911,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1646,7 +1920,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1655,12 +1929,14 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1683,24 +1959,24 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="6"/>
-    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.90625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.81640625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="6"/>
+    <col min="1" max="1" width="8.796875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.53125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.1328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.796875" style="6"/>
+    <col min="9" max="9" width="26.73046875" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1711,7 +1987,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="B2" s="24" t="s">
         <v>31</v>
       </c>
@@ -1726,7 +2002,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1737,7 +2013,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
@@ -1753,7 +2029,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -1765,7 +2041,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -1774,7 +2050,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1791,36 +2067,56 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="35.65" customHeight="1">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="39.4" customHeight="1">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>59</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="38.65" customHeight="1">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1830,7 +2126,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1840,7 +2136,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1850,7 +2146,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1860,7 +2156,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1870,7 +2166,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1880,7 +2176,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1890,7 +2186,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1900,7 +2196,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1910,7 +2206,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1920,7 +2216,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1930,7 +2226,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1940,7 +2236,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1950,7 +2246,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1960,7 +2256,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1970,7 +2266,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1980,7 +2276,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1990,7 +2286,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2000,7 +2296,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6">
       <c r="C32" s="34" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
modified the code according to suggestions
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8775474af38bcd54/Desktop/anul3/VVSS/VVSS-labs/Docs/Lab01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daria\OneDrive\Desktop\VVSS-labs\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{99F4FD46-6DA1-44A7-A17B-8F11551B1C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80B598AF-E07D-4100-A9B9-D5F34FD486CA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F85A13-0CE8-4B32-8FFE-8DC225A1FD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="650" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -19,24 +19,11 @@
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -179,83 +166,16 @@
     <t xml:space="preserve">Nu, lipsesc majoritatea </t>
   </si>
   <si>
-    <t>C04</t>
-  </si>
-  <si>
     <t>C08</t>
   </si>
   <si>
     <t>C06</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">gestionarea excepțiilor pentru </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IOException</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> cu </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>e.printStackTrace();</t>
-    </r>
-  </si>
-  <si>
     <t>C03</t>
   </si>
   <si>
     <t>In Kitchen GUI Controller avem un while (true) care ar putea fi inlocuit</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Metoda </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>getPayment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> nu validează formatul datelor din fișier. Dacă linia citită nu respectă formatul așteptat, pot rezulta excepții runtime</t>
-    </r>
-  </si>
-  <si>
-    <t>Dacă structura fișierelDor se schimbă sau dacă există erori în datele de intrare, codul actual nu trateaza aceste probleme într-un mod care să împiedice crash-ul aplicației sau erori de runtime. Ar trebui să existe validări ale formatului datelor citite.</t>
   </si>
   <si>
     <t>OrdersGUIController, 53</t>
@@ -374,12 +294,30 @@
   <si>
     <t>PAymentAlert</t>
   </si>
+  <si>
+    <t>Gestionarea excepțiilor pentru IOException cu e.printStackTrace();</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Metoda </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>getPayment nu validează formatul datelor din fișier. Dacă linia citită nu respectă formatul așteptat, pot rezulta excepții runtime</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,30 +403,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FFBCBEC4"/>
       <name val="JetBrains Mono"/>
@@ -505,6 +419,13 @@
       <color rgb="FF56A8F5"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -606,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -637,6 +558,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -678,17 +608,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,40 +922,40 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.796875" style="6"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.36328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.36328125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.796875" style="6"/>
+    <col min="10" max="10" width="14.36328125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1060,10 +979,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1078,10 +997,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1093,15 +1012,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1117,7 +1036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="43.5">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1125,11 +1044,11 @@
         <v>36</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="43.5">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1138,11 +1057,11 @@
         <v>35</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="72.5">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1151,7 +1070,7 @@
         <v>37</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1302,39 +1221,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.796875" style="6"/>
-    <col min="9" max="9" width="22.06640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.796875" style="6"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.36328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.36328125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="6"/>
+    <col min="9" max="9" width="22.08984375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1358,10 +1277,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1376,10 +1295,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1391,15 +1310,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1415,7 +1334,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="43.5">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1423,11 +1342,11 @@
         <v>41</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="29">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1436,7 +1355,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1607,42 +1526,42 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.796875" style="6"/>
-    <col min="9" max="9" width="26.73046875" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.796875" style="6"/>
+    <col min="5" max="5" width="41.36328125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="6"/>
+    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1666,10 +1585,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1684,10 +1603,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1699,15 +1618,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1723,63 +1642,59 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="29">
       <c r="B10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="D10" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:10" ht="43.5">
       <c r="B11" s="3">
-        <f>B10+1</f>
-        <v>2</v>
+        <f t="shared" ref="B11:B29" si="0">B10+1</f>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11"/>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29">
       <c r="B12" s="3">
-        <f t="shared" ref="B12:B30" si="0">B11+1</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.5">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
@@ -1788,7 +1703,7 @@
     <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
@@ -1797,7 +1712,7 @@
     <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
@@ -1806,7 +1721,7 @@
     <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
@@ -1815,43 +1730,43 @@
     <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
@@ -1860,7 +1775,7 @@
     <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
@@ -1869,7 +1784,7 @@
     <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
@@ -1878,34 +1793,34 @@
     <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
@@ -1914,27 +1829,18 @@
     <row r="29" spans="2:5">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="3">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="C32" s="11" t="s">
+    <row r="31" spans="2:5">
+      <c r="C31" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="1">
+      <c r="D31" s="12"/>
+      <c r="E31" s="1">
         <v>0.5</v>
       </c>
     </row>
@@ -1959,41 +1865,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.53125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.1328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.59765625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.796875" style="6"/>
-    <col min="9" max="9" width="26.73046875" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.796875" style="6"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.08984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.81640625" style="6"/>
+    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -2017,8 +1923,8 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2033,8 +1939,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2046,8 +1952,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10">
@@ -2072,16 +1978,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="39.4" customHeight="1">
@@ -2090,13 +1996,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -2106,13 +2012,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="40" t="s">
         <v>60</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>56</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -2297,11 +2203,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>